<commit_message>
.gitignore is now working
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata.xlsx
+++ b/src/test/resources/testdata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6555" tabRatio="829" firstSheet="1" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6555" tabRatio="829" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="RunManager" sheetId="1" r:id="rId1"/>
@@ -4047,7 +4047,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4496,7 +4496,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -9008,8 +9008,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="15"/>

</xml_diff>